<commit_message>
update settling velocity calculations for paper outline
</commit_message>
<xml_diff>
--- a/Suspended_Sediment_Analysis/settling_velocity/settling_velocity_calculation.xlsx
+++ b/Suspended_Sediment_Analysis/settling_velocity/settling_velocity_calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Suspended_Sediment_Analysis\settling_velocity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76860313-0A10-454A-9D4D-FE6F3F5D3881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B42549-546A-4C65-839E-DC826235D4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5725,8 +5725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M47" sqref="M47"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>